<commit_message>
Fix for AWACS ground collisions
</commit_message>
<xml_diff>
--- a/DOC/navpoints-w MGRS.xlsx
+++ b/DOC/navpoints-w MGRS.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$525</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3219" uniqueCount="2864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3226" uniqueCount="2870">
   <si>
     <t>ACOSU</t>
   </si>
@@ -8606,13 +8609,31 @@
   </si>
   <si>
     <t>114°51'03"</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>TACAN/BRG</t>
+  </si>
+  <si>
+    <t>GPRS</t>
+  </si>
+  <si>
+    <t>LAT</t>
+  </si>
+  <si>
+    <t>LONG</t>
+  </si>
+  <si>
+    <t>LNG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8625,6 +8646,13 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -8694,7 +8722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -8720,6 +8748,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9024,12 +9053,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G525"/>
+  <dimension ref="A1:G525"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C527" sqref="C527"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>2864</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>2865</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2866</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2867</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>2868</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>2867</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>2869</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>0</v>
@@ -20185,6 +20239,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G525"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>

</xml_diff>